<commit_message>
add prototypes, design class diagrams and plan, etc
</commit_message>
<xml_diff>
--- a/Elaboration Third Phase Plan.xlsx
+++ b/Elaboration Third Phase Plan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\Object Oriented Design\Project\Docs\OOD_Project_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A220F0-FFDF-489C-8FE7-F8977A349E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D124F083-4AC7-4C45-BD77-E1F4B5FDC8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
   <si>
     <t>Alireza B</t>
   </si>
@@ -184,13 +185,112 @@
   </si>
   <si>
     <t>اتمام کد baseline و پیاده سازی ریسک به همراه آپدیت سایر محصولات</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Diagrams</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>خرید محتوا</t>
+  </si>
+  <si>
+    <t>10 درصد سهم قاصدک</t>
+  </si>
+  <si>
+    <t>ادیت جزئیات کانال</t>
+  </si>
+  <si>
+    <t>facade</t>
+  </si>
+  <si>
+    <t>از صفر تا صد</t>
+  </si>
+  <si>
+    <t>اعمال تو طراحی</t>
+  </si>
+  <si>
+    <t>غیرفعال کردن اشتراک</t>
+  </si>
+  <si>
+    <t>کنسل کردن</t>
+  </si>
+  <si>
+    <t>ساجسشن و سرچ</t>
+  </si>
+  <si>
+    <t>تحلیل</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>آپدیت</t>
+  </si>
+  <si>
+    <t>حذف کانال</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> برداشت وجه از کیف پول</t>
+  </si>
+  <si>
+    <t>افزودن محتوا به کانال</t>
+  </si>
+  <si>
+    <t>سازگاری محتواها در کانال</t>
+  </si>
+  <si>
+    <t>رجیستر</t>
+  </si>
+  <si>
+    <t>ایجی</t>
+  </si>
+  <si>
+    <t>Sequences</t>
+  </si>
+  <si>
+    <t>4 تا دسته بندی</t>
+  </si>
+  <si>
+    <t>3 تا مالی</t>
+  </si>
+  <si>
+    <t>افزودن مدیر</t>
+  </si>
+  <si>
+    <t>حذف  کاربر</t>
+  </si>
+  <si>
+    <t>حذف مدیر</t>
+  </si>
+  <si>
+    <t>4 تا محتوا</t>
+  </si>
+  <si>
+    <t>لیست محتوا</t>
+  </si>
+  <si>
+    <t>2 تا جست و جو</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 تا واکنش </t>
+  </si>
+  <si>
+    <t>تایم لاین</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,8 +341,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +378,21 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -330,14 +466,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
@@ -363,15 +502,54 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="5" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="7" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment readingOrder="2"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="8">
+    <cellStyle name="Bad" xfId="6" builtinId="27"/>
+    <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
+    <cellStyle name="Neutral" xfId="7" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
@@ -655,39 +833,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:10" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="9"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" ht="14.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
@@ -706,10 +884,10 @@
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
@@ -728,10 +906,10 @@
       <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="8" t="s">
         <v>18</v>
       </c>
@@ -750,10 +928,10 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="8" t="s">
         <v>34</v>
       </c>
@@ -772,10 +950,10 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="8" t="s">
         <v>35</v>
       </c>
@@ -794,10 +972,10 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="8" t="s">
         <v>24</v>
       </c>
@@ -816,10 +994,10 @@
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="8" t="s">
         <v>25</v>
       </c>
@@ -1018,4 +1196,471 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27707C41-AEFA-43F8-B625-D60B12AAAA79}">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.3984375" customWidth="1"/>
+    <col min="2" max="2" width="21.19921875" customWidth="1"/>
+    <col min="3" max="3" width="18.9296875" customWidth="1"/>
+    <col min="4" max="4" width="24.9296875" customWidth="1"/>
+    <col min="5" max="5" width="27.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>